<commit_message>
planning update en rename van en bestand
</commit_message>
<xml_diff>
--- a/Algemene planning.xlsx
+++ b/Algemene planning.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
   <si>
     <t>GroepsProject Robotica</t>
   </si>
@@ -127,13 +127,25 @@
   </si>
   <si>
     <t>Vergadering agenda's netjes maken + notulen overnemen van aantekeningen</t>
+  </si>
+  <si>
+    <t>Rollenverdeling met uitleg van waarom een rol is gekozen binnen het team op internet zetten. Met link naar de Belbin test.</t>
+  </si>
+  <si>
+    <t>Voortgangsvergadering</t>
+  </si>
+  <si>
+    <t>Activity diagrams maken</t>
+  </si>
+  <si>
+    <t>Use case diagram maken</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -158,8 +170,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,6 +213,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -224,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -284,6 +307,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -617,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -895,7 +920,7 @@
       <c r="B28" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="27" t="s">
         <v>24</v>
       </c>
     </row>
@@ -906,7 +931,7 @@
       <c r="B29" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="13" t="s">
         <v>30</v>
       </c>
     </row>
@@ -917,7 +942,7 @@
       <c r="B30" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="13" t="s">
         <v>31</v>
       </c>
     </row>
@@ -928,7 +953,7 @@
       <c r="B31" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="13" t="s">
         <v>32</v>
       </c>
     </row>
@@ -939,7 +964,7 @@
       <c r="B32" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="13" t="s">
         <v>33</v>
       </c>
     </row>
@@ -950,7 +975,7 @@
       <c r="B33" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="21" t="s">
         <v>35</v>
       </c>
     </row>
@@ -961,7 +986,9 @@
       <c r="B34" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C34" s="7"/>
+      <c r="C34" s="21" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="5">
@@ -970,7 +997,9 @@
       <c r="B35" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="7"/>
+      <c r="C35" s="21" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="5">
@@ -979,7 +1008,7 @@
       <c r="B36" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="21" t="s">
         <v>34</v>
       </c>
     </row>
@@ -990,7 +1019,9 @@
       <c r="B37" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="7"/>
+      <c r="C37" s="26" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="5">
@@ -999,7 +1030,9 @@
       <c r="B38" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="7"/>
+      <c r="C38" s="26" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="5">
@@ -1008,7 +1041,7 @@
       <c r="B39" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="7"/>
+      <c r="C39" s="26"/>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="5">
@@ -1017,7 +1050,7 @@
       <c r="B40" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C40" s="7"/>
+      <c r="C40" s="26"/>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="5">
@@ -1026,7 +1059,7 @@
       <c r="B41" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="7"/>
+      <c r="C41" s="26"/>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="5">
@@ -1035,7 +1068,7 @@
       <c r="B42" s="6">
         <v>42461</v>
       </c>
-      <c r="C42" s="7"/>
+      <c r="C42" s="28"/>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="5">
@@ -1044,7 +1077,7 @@
       <c r="B43" s="6">
         <v>42461</v>
       </c>
-      <c r="C43" s="7"/>
+      <c r="C43" s="28"/>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="5">
@@ -1053,7 +1086,7 @@
       <c r="B44" s="6">
         <v>42461</v>
       </c>
-      <c r="C44" s="7"/>
+      <c r="C44" s="28"/>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="5">
@@ -1062,7 +1095,7 @@
       <c r="B45" s="6">
         <v>42461</v>
       </c>
-      <c r="C45" s="7"/>
+      <c r="C45" s="28"/>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="5">
@@ -1071,7 +1104,7 @@
       <c r="B46" s="6">
         <v>42461</v>
       </c>
-      <c r="C46" s="7"/>
+      <c r="C46" s="28"/>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="8"/>

</xml_diff>